<commit_message>
add reviews label dataset sample
</commit_message>
<xml_diff>
--- a/data/processed/sentiment_analysis_reviews_label.xlsx
+++ b/data/processed/sentiment_analysis_reviews_label.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University of Michigan\Courses\SIADS 697 &amp; 698 Capstone\Realtime Dreamer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heyun\Capstone\realtime-dreamer\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E76BA9-64B5-4C21-B0EE-AAA322369959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F4E746-0EC6-40FF-9129-213A4F11F1B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{3D2ECFB1-7ED4-4F8E-A3AB-AE95FDA978B4}"/>
   </bookViews>
@@ -1086,7 +1086,7 @@
   <dimension ref="A1:D201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A3" sqref="A3:A201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1110,7 +1110,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
-        <v>160</v>
+        <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>7</v>
@@ -1124,7 +1124,8 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
-        <v>332</v>
+        <f>A2+1</f>
+        <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>5</v>
@@ -1138,7 +1139,8 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
-        <v>394</v>
+        <f t="shared" ref="A4:A67" si="0">A3+1</f>
+        <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>4</v>
@@ -1152,7 +1154,8 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
-        <v>910</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>6</v>
@@ -1166,7 +1169,8 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
-        <v>5693</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>205</v>
@@ -1180,7 +1184,8 @@
     </row>
     <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
-        <v>5690</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>206</v>
@@ -1194,7 +1199,8 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>74</v>
@@ -1208,7 +1214,8 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>54</v>
@@ -1222,7 +1229,8 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>131</v>
@@ -1236,7 +1244,8 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>136</v>
@@ -1250,7 +1259,8 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>77</v>
@@ -1264,7 +1274,8 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>132</v>
@@ -1278,7 +1289,8 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>87</v>
@@ -1292,7 +1304,8 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>89</v>
@@ -1306,7 +1319,8 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
-        <v>9</v>
+        <f t="shared" si="0"/>
+        <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>14</v>
@@ -1320,7 +1334,8 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>73</v>
@@ -1334,7 +1349,8 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>169</v>
@@ -1348,7 +1364,8 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
-        <v>12</v>
+        <f t="shared" si="0"/>
+        <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>129</v>
@@ -1362,7 +1379,8 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
-        <v>13</v>
+        <f t="shared" si="0"/>
+        <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>175</v>
@@ -1376,7 +1394,8 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
-        <v>14</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>152</v>
@@ -1390,7 +1409,8 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
-        <v>15</v>
+        <f t="shared" si="0"/>
+        <v>21</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>202</v>
@@ -1404,7 +1424,8 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
-        <v>16</v>
+        <f t="shared" si="0"/>
+        <v>22</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>194</v>
@@ -1418,7 +1439,8 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
-        <v>31</v>
+        <f t="shared" si="0"/>
+        <v>23</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>110</v>
@@ -1432,7 +1454,8 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
-        <v>32</v>
+        <f t="shared" si="0"/>
+        <v>24</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>108</v>
@@ -1446,7 +1469,8 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
-        <v>33</v>
+        <f t="shared" si="0"/>
+        <v>25</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>166</v>
@@ -1460,7 +1484,8 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
-        <v>34</v>
+        <f t="shared" si="0"/>
+        <v>26</v>
       </c>
       <c r="B27" s="10" t="s">
         <v>113</v>
@@ -1474,7 +1499,8 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
-        <v>61</v>
+        <f t="shared" si="0"/>
+        <v>27</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>107</v>
@@ -1488,7 +1514,8 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
-        <v>62</v>
+        <f t="shared" si="0"/>
+        <v>28</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>69</v>
@@ -1502,7 +1529,8 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
-        <v>63</v>
+        <f t="shared" si="0"/>
+        <v>29</v>
       </c>
       <c r="B30" s="10" t="s">
         <v>96</v>
@@ -1516,7 +1544,8 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
-        <v>64</v>
+        <f t="shared" si="0"/>
+        <v>30</v>
       </c>
       <c r="B31" s="10" t="s">
         <v>195</v>
@@ -1530,7 +1559,8 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
-        <v>65</v>
+        <f t="shared" si="0"/>
+        <v>31</v>
       </c>
       <c r="B32" s="10" t="s">
         <v>203</v>
@@ -1544,7 +1574,8 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
-        <v>66</v>
+        <f t="shared" si="0"/>
+        <v>32</v>
       </c>
       <c r="B33" s="10" t="s">
         <v>90</v>
@@ -1558,7 +1589,8 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
-        <v>67</v>
+        <f t="shared" si="0"/>
+        <v>33</v>
       </c>
       <c r="B34" s="10" t="s">
         <v>88</v>
@@ -1572,7 +1604,8 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
-        <v>68</v>
+        <f t="shared" si="0"/>
+        <v>34</v>
       </c>
       <c r="B35" s="10" t="s">
         <v>150</v>
@@ -1586,7 +1619,8 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
-        <v>69</v>
+        <f t="shared" si="0"/>
+        <v>35</v>
       </c>
       <c r="B36" s="9" t="s">
         <v>22</v>
@@ -1600,7 +1634,8 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
-        <v>70</v>
+        <f t="shared" si="0"/>
+        <v>36</v>
       </c>
       <c r="B37" s="10" t="s">
         <v>193</v>
@@ -1614,7 +1649,8 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
-        <v>71</v>
+        <f t="shared" si="0"/>
+        <v>37</v>
       </c>
       <c r="B38" s="10" t="s">
         <v>92</v>
@@ -1628,7 +1664,8 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
-        <v>72</v>
+        <f t="shared" si="0"/>
+        <v>38</v>
       </c>
       <c r="B39" s="10" t="s">
         <v>177</v>
@@ -1642,7 +1679,8 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
-        <v>73</v>
+        <f t="shared" si="0"/>
+        <v>39</v>
       </c>
       <c r="B40" s="10" t="s">
         <v>114</v>
@@ -1656,7 +1694,8 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
-        <v>74</v>
+        <f t="shared" si="0"/>
+        <v>40</v>
       </c>
       <c r="B41" s="10" t="s">
         <v>139</v>
@@ -1670,7 +1709,8 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
-        <v>75</v>
+        <f t="shared" si="0"/>
+        <v>41</v>
       </c>
       <c r="B42" s="10" t="s">
         <v>137</v>
@@ -1684,7 +1724,8 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
-        <v>76</v>
+        <f t="shared" si="0"/>
+        <v>42</v>
       </c>
       <c r="B43" s="10" t="s">
         <v>187</v>
@@ -1698,7 +1739,8 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
-        <v>85</v>
+        <f t="shared" si="0"/>
+        <v>43</v>
       </c>
       <c r="B44" s="10" t="s">
         <v>148</v>
@@ -1712,7 +1754,8 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
-        <v>104</v>
+        <f t="shared" si="0"/>
+        <v>44</v>
       </c>
       <c r="B45" s="10" t="s">
         <v>81</v>
@@ -1726,7 +1769,8 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
-        <v>105</v>
+        <f t="shared" si="0"/>
+        <v>45</v>
       </c>
       <c r="B46" s="10" t="s">
         <v>171</v>
@@ -1740,7 +1784,8 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
-        <v>106</v>
+        <f t="shared" si="0"/>
+        <v>46</v>
       </c>
       <c r="B47" s="9" t="s">
         <v>31</v>
@@ -1754,7 +1799,8 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
-        <v>107</v>
+        <f t="shared" si="0"/>
+        <v>47</v>
       </c>
       <c r="B48" s="10" t="s">
         <v>163</v>
@@ -1768,7 +1814,8 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
-        <v>108</v>
+        <f t="shared" si="0"/>
+        <v>48</v>
       </c>
       <c r="B49" s="9" t="s">
         <v>52</v>
@@ -1782,7 +1829,8 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
-        <v>109</v>
+        <f t="shared" si="0"/>
+        <v>49</v>
       </c>
       <c r="B50" s="9" t="s">
         <v>43</v>
@@ -1796,7 +1844,8 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
-        <v>110</v>
+        <f t="shared" si="0"/>
+        <v>50</v>
       </c>
       <c r="B51" s="9" t="s">
         <v>9</v>
@@ -1810,7 +1859,8 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
-        <v>111</v>
+        <f t="shared" si="0"/>
+        <v>51</v>
       </c>
       <c r="B52" s="9" t="s">
         <v>37</v>
@@ -1824,7 +1874,8 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
-        <v>112</v>
+        <f t="shared" si="0"/>
+        <v>52</v>
       </c>
       <c r="B53" s="10" t="s">
         <v>106</v>
@@ -1838,7 +1889,8 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
-        <v>113</v>
+        <f t="shared" si="0"/>
+        <v>53</v>
       </c>
       <c r="B54" s="9" t="s">
         <v>16</v>
@@ -1852,7 +1904,8 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
-        <v>114</v>
+        <f t="shared" si="0"/>
+        <v>54</v>
       </c>
       <c r="B55" s="9" t="s">
         <v>10</v>
@@ -1866,7 +1919,8 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
-        <v>115</v>
+        <f t="shared" si="0"/>
+        <v>55</v>
       </c>
       <c r="B56" s="10" t="s">
         <v>68</v>
@@ -1880,7 +1934,8 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
-        <v>116</v>
+        <f t="shared" si="0"/>
+        <v>56</v>
       </c>
       <c r="B57" s="10" t="s">
         <v>98</v>
@@ -1894,7 +1949,8 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
-        <v>117</v>
+        <f t="shared" si="0"/>
+        <v>57</v>
       </c>
       <c r="B58" s="9" t="s">
         <v>36</v>
@@ -1908,7 +1964,8 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
-        <v>118</v>
+        <f t="shared" si="0"/>
+        <v>58</v>
       </c>
       <c r="B59" s="10" t="s">
         <v>118</v>
@@ -1922,7 +1979,8 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
-        <v>119</v>
+        <f t="shared" si="0"/>
+        <v>59</v>
       </c>
       <c r="B60" s="9" t="s">
         <v>35</v>
@@ -1936,7 +1994,8 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
-        <v>120</v>
+        <f t="shared" si="0"/>
+        <v>60</v>
       </c>
       <c r="B61" s="10" t="s">
         <v>185</v>
@@ -1950,7 +2009,8 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
-        <v>121</v>
+        <f t="shared" si="0"/>
+        <v>61</v>
       </c>
       <c r="B62" s="9" t="s">
         <v>27</v>
@@ -1964,7 +2024,8 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
-        <v>122</v>
+        <f t="shared" si="0"/>
+        <v>62</v>
       </c>
       <c r="B63" s="10" t="s">
         <v>78</v>
@@ -1978,7 +2039,8 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
-        <v>123</v>
+        <f t="shared" si="0"/>
+        <v>63</v>
       </c>
       <c r="B64" s="9" t="s">
         <v>32</v>
@@ -1992,7 +2054,8 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
-        <v>124</v>
+        <f t="shared" si="0"/>
+        <v>64</v>
       </c>
       <c r="B65" s="10" t="s">
         <v>97</v>
@@ -2006,7 +2069,8 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
-        <v>125</v>
+        <f t="shared" si="0"/>
+        <v>65</v>
       </c>
       <c r="B66" s="10" t="s">
         <v>164</v>
@@ -2020,7 +2084,8 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
-        <v>126</v>
+        <f t="shared" si="0"/>
+        <v>66</v>
       </c>
       <c r="B67" s="10" t="s">
         <v>201</v>
@@ -2034,7 +2099,8 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
-        <v>127</v>
+        <f t="shared" ref="A68:A131" si="1">A67+1</f>
+        <v>67</v>
       </c>
       <c r="B68" s="10" t="s">
         <v>105</v>
@@ -2048,7 +2114,8 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
-        <v>128</v>
+        <f t="shared" si="1"/>
+        <v>68</v>
       </c>
       <c r="B69" s="10" t="s">
         <v>140</v>
@@ -2062,7 +2129,8 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="3">
-        <v>129</v>
+        <f t="shared" si="1"/>
+        <v>69</v>
       </c>
       <c r="B70" s="10" t="s">
         <v>170</v>
@@ -2076,7 +2144,8 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
-        <v>130</v>
+        <f t="shared" si="1"/>
+        <v>70</v>
       </c>
       <c r="B71" s="10" t="s">
         <v>75</v>
@@ -2090,7 +2159,8 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="3">
-        <v>131</v>
+        <f t="shared" si="1"/>
+        <v>71</v>
       </c>
       <c r="B72" s="10" t="s">
         <v>162</v>
@@ -2104,7 +2174,8 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="3">
-        <v>132</v>
+        <f t="shared" si="1"/>
+        <v>72</v>
       </c>
       <c r="B73" s="10" t="s">
         <v>101</v>
@@ -2118,7 +2189,8 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="3">
-        <v>133</v>
+        <f t="shared" si="1"/>
+        <v>73</v>
       </c>
       <c r="B74" s="10" t="s">
         <v>135</v>
@@ -2132,7 +2204,8 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="3">
-        <v>136</v>
+        <f t="shared" si="1"/>
+        <v>74</v>
       </c>
       <c r="B75" s="10" t="s">
         <v>143</v>
@@ -2146,7 +2219,8 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
-        <v>137</v>
+        <f t="shared" si="1"/>
+        <v>75</v>
       </c>
       <c r="B76" s="10" t="s">
         <v>93</v>
@@ -2160,7 +2234,8 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
-        <v>138</v>
+        <f t="shared" si="1"/>
+        <v>76</v>
       </c>
       <c r="B77" s="10" t="s">
         <v>112</v>
@@ -2174,7 +2249,8 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="3">
-        <v>139</v>
+        <f t="shared" si="1"/>
+        <v>77</v>
       </c>
       <c r="B78" s="10" t="s">
         <v>138</v>
@@ -2188,7 +2264,8 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="3">
-        <v>142</v>
+        <f t="shared" si="1"/>
+        <v>78</v>
       </c>
       <c r="B79" s="10" t="s">
         <v>111</v>
@@ -2202,7 +2279,8 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="3">
-        <v>144</v>
+        <f t="shared" si="1"/>
+        <v>79</v>
       </c>
       <c r="B80" s="9" t="s">
         <v>56</v>
@@ -2216,7 +2294,8 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="3">
-        <v>145</v>
+        <f t="shared" si="1"/>
+        <v>80</v>
       </c>
       <c r="B81" s="9" t="s">
         <v>24</v>
@@ -2230,7 +2309,8 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="3">
-        <v>146</v>
+        <f t="shared" si="1"/>
+        <v>81</v>
       </c>
       <c r="B82" s="8" t="s">
         <v>144</v>
@@ -2244,7 +2324,8 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="3">
-        <v>147</v>
+        <f t="shared" si="1"/>
+        <v>82</v>
       </c>
       <c r="B83" s="9" t="s">
         <v>50</v>
@@ -2258,7 +2339,8 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="3">
-        <v>148</v>
+        <f t="shared" si="1"/>
+        <v>83</v>
       </c>
       <c r="B84" s="9" t="s">
         <v>42</v>
@@ -2272,7 +2354,8 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="3">
-        <v>149</v>
+        <f t="shared" si="1"/>
+        <v>84</v>
       </c>
       <c r="B85" s="9" t="s">
         <v>49</v>
@@ -2286,7 +2369,8 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="3">
-        <v>150</v>
+        <f t="shared" si="1"/>
+        <v>85</v>
       </c>
       <c r="B86" s="10" t="s">
         <v>109</v>
@@ -2300,7 +2384,8 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="3">
-        <v>152</v>
+        <f t="shared" si="1"/>
+        <v>86</v>
       </c>
       <c r="B87" s="10" t="s">
         <v>71</v>
@@ -2314,7 +2399,8 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="3">
-        <v>153</v>
+        <f t="shared" si="1"/>
+        <v>87</v>
       </c>
       <c r="B88" s="10" t="s">
         <v>192</v>
@@ -2328,7 +2414,8 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="3">
-        <v>155</v>
+        <f t="shared" si="1"/>
+        <v>88</v>
       </c>
       <c r="B89" s="9" t="s">
         <v>39</v>
@@ -2342,7 +2429,8 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="3">
-        <v>157</v>
+        <f t="shared" si="1"/>
+        <v>89</v>
       </c>
       <c r="B90" s="10" t="s">
         <v>198</v>
@@ -2356,7 +2444,8 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="3">
-        <v>158</v>
+        <f t="shared" si="1"/>
+        <v>90</v>
       </c>
       <c r="B91" s="9" t="s">
         <v>26</v>
@@ -2370,7 +2459,8 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="3">
-        <v>159</v>
+        <f t="shared" si="1"/>
+        <v>91</v>
       </c>
       <c r="B92" s="10" t="s">
         <v>82</v>
@@ -2384,7 +2474,8 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="3">
-        <v>160</v>
+        <f t="shared" si="1"/>
+        <v>92</v>
       </c>
       <c r="B93" s="10" t="s">
         <v>83</v>
@@ -2398,7 +2489,8 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="3">
-        <v>161</v>
+        <f t="shared" si="1"/>
+        <v>93</v>
       </c>
       <c r="B94" s="10" t="s">
         <v>84</v>
@@ -2412,7 +2504,8 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="3">
-        <v>162</v>
+        <f t="shared" si="1"/>
+        <v>94</v>
       </c>
       <c r="B95" s="10" t="s">
         <v>80</v>
@@ -2426,7 +2519,8 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="3">
-        <v>163</v>
+        <f t="shared" si="1"/>
+        <v>95</v>
       </c>
       <c r="B96" s="10" t="s">
         <v>142</v>
@@ -2440,7 +2534,8 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="3">
-        <v>164</v>
+        <f t="shared" si="1"/>
+        <v>96</v>
       </c>
       <c r="B97" s="10" t="s">
         <v>200</v>
@@ -2454,7 +2549,8 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="3">
-        <v>165</v>
+        <f t="shared" si="1"/>
+        <v>97</v>
       </c>
       <c r="B98" s="10" t="s">
         <v>199</v>
@@ -2468,7 +2564,8 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="3">
-        <v>166</v>
+        <f t="shared" si="1"/>
+        <v>98</v>
       </c>
       <c r="B99" s="10" t="s">
         <v>125</v>
@@ -2482,7 +2579,8 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="3">
-        <v>167</v>
+        <f t="shared" si="1"/>
+        <v>99</v>
       </c>
       <c r="B100" s="9" t="s">
         <v>46</v>
@@ -2496,7 +2594,8 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="3">
-        <v>169</v>
+        <f t="shared" si="1"/>
+        <v>100</v>
       </c>
       <c r="B101" s="10" t="s">
         <v>134</v>
@@ -2510,7 +2609,8 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="3">
-        <v>170</v>
+        <f t="shared" si="1"/>
+        <v>101</v>
       </c>
       <c r="B102" s="10" t="s">
         <v>116</v>
@@ -2524,7 +2624,8 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="3">
-        <v>171</v>
+        <f t="shared" si="1"/>
+        <v>102</v>
       </c>
       <c r="B103" s="10" t="s">
         <v>115</v>
@@ -2538,7 +2639,8 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="3">
-        <v>174</v>
+        <f t="shared" si="1"/>
+        <v>103</v>
       </c>
       <c r="B104" s="10" t="s">
         <v>122</v>
@@ -2552,7 +2654,8 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="3">
-        <v>175</v>
+        <f t="shared" si="1"/>
+        <v>104</v>
       </c>
       <c r="B105" s="10" t="s">
         <v>165</v>
@@ -2566,7 +2669,8 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="3">
-        <v>176</v>
+        <f t="shared" si="1"/>
+        <v>105</v>
       </c>
       <c r="B106" s="9" t="s">
         <v>55</v>
@@ -2580,7 +2684,8 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="3">
-        <v>177</v>
+        <f t="shared" si="1"/>
+        <v>106</v>
       </c>
       <c r="B107" s="10" t="s">
         <v>100</v>
@@ -2594,7 +2699,8 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="3">
-        <v>178</v>
+        <f t="shared" si="1"/>
+        <v>107</v>
       </c>
       <c r="B108" s="10" t="s">
         <v>191</v>
@@ -2608,7 +2714,8 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="3">
-        <v>179</v>
+        <f t="shared" si="1"/>
+        <v>108</v>
       </c>
       <c r="B109" s="9" t="s">
         <v>28</v>
@@ -2622,7 +2729,8 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="3">
-        <v>180</v>
+        <f t="shared" si="1"/>
+        <v>109</v>
       </c>
       <c r="B110" s="9" t="s">
         <v>48</v>
@@ -2636,7 +2744,8 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="3">
-        <v>181</v>
+        <f t="shared" si="1"/>
+        <v>110</v>
       </c>
       <c r="B111" s="9" t="s">
         <v>44</v>
@@ -2650,7 +2759,8 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="3">
-        <v>182</v>
+        <f t="shared" si="1"/>
+        <v>111</v>
       </c>
       <c r="B112" s="10" t="s">
         <v>95</v>
@@ -2664,7 +2774,8 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="3">
-        <v>183</v>
+        <f t="shared" si="1"/>
+        <v>112</v>
       </c>
       <c r="B113" s="10" t="s">
         <v>94</v>
@@ -2678,7 +2789,8 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="3">
-        <v>184</v>
+        <f t="shared" si="1"/>
+        <v>113</v>
       </c>
       <c r="B114" s="10" t="s">
         <v>174</v>
@@ -2692,7 +2804,8 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="3">
-        <v>185</v>
+        <f t="shared" si="1"/>
+        <v>114</v>
       </c>
       <c r="B115" s="9" t="s">
         <v>38</v>
@@ -2706,7 +2819,8 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="3">
-        <v>186</v>
+        <f t="shared" si="1"/>
+        <v>115</v>
       </c>
       <c r="B116" s="9" t="s">
         <v>40</v>
@@ -2720,7 +2834,8 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="3">
-        <v>187</v>
+        <f t="shared" si="1"/>
+        <v>116</v>
       </c>
       <c r="B117" s="10" t="s">
         <v>124</v>
@@ -2734,7 +2849,8 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="3">
-        <v>188</v>
+        <f t="shared" si="1"/>
+        <v>117</v>
       </c>
       <c r="B118" s="10" t="s">
         <v>188</v>
@@ -2748,7 +2864,8 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="3">
-        <v>189</v>
+        <f t="shared" si="1"/>
+        <v>118</v>
       </c>
       <c r="B119" s="10" t="s">
         <v>189</v>
@@ -2762,7 +2879,8 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="3">
-        <v>190</v>
+        <f t="shared" si="1"/>
+        <v>119</v>
       </c>
       <c r="B120" s="10" t="s">
         <v>186</v>
@@ -2776,7 +2894,8 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="3">
-        <v>191</v>
+        <f t="shared" si="1"/>
+        <v>120</v>
       </c>
       <c r="B121" s="9" t="s">
         <v>20</v>
@@ -2790,7 +2909,8 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="3">
-        <v>192</v>
+        <f t="shared" si="1"/>
+        <v>121</v>
       </c>
       <c r="B122" s="10" t="s">
         <v>158</v>
@@ -2804,7 +2924,8 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="3">
-        <v>193</v>
+        <f t="shared" si="1"/>
+        <v>122</v>
       </c>
       <c r="B123" s="10" t="s">
         <v>160</v>
@@ -2818,7 +2939,8 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="3">
-        <v>194</v>
+        <f t="shared" si="1"/>
+        <v>123</v>
       </c>
       <c r="B124" s="10" t="s">
         <v>70</v>
@@ -2832,7 +2954,8 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="3">
-        <v>195</v>
+        <f t="shared" si="1"/>
+        <v>124</v>
       </c>
       <c r="B125" s="10" t="s">
         <v>76</v>
@@ -2846,7 +2969,8 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="3">
-        <v>196</v>
+        <f t="shared" si="1"/>
+        <v>125</v>
       </c>
       <c r="B126" s="10" t="s">
         <v>117</v>
@@ -2860,7 +2984,8 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="3">
-        <v>197</v>
+        <f t="shared" si="1"/>
+        <v>126</v>
       </c>
       <c r="B127" s="10" t="s">
         <v>159</v>
@@ -2874,7 +2999,8 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="3">
-        <v>198</v>
+        <f t="shared" si="1"/>
+        <v>127</v>
       </c>
       <c r="B128" s="10" t="s">
         <v>86</v>
@@ -2888,7 +3014,8 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="3">
-        <v>199</v>
+        <f t="shared" si="1"/>
+        <v>128</v>
       </c>
       <c r="B129" s="10" t="s">
         <v>102</v>
@@ -2902,7 +3029,8 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="3">
-        <v>200</v>
+        <f t="shared" si="1"/>
+        <v>129</v>
       </c>
       <c r="B130" s="9" t="s">
         <v>13</v>
@@ -2916,7 +3044,8 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="3">
-        <v>201</v>
+        <f t="shared" si="1"/>
+        <v>130</v>
       </c>
       <c r="B131" s="10" t="s">
         <v>197</v>
@@ -2930,7 +3059,8 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="3">
-        <v>202</v>
+        <f t="shared" ref="A132:A195" si="2">A131+1</f>
+        <v>131</v>
       </c>
       <c r="B132" s="9" t="s">
         <v>17</v>
@@ -2944,7 +3074,8 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="3">
-        <v>203</v>
+        <f t="shared" si="2"/>
+        <v>132</v>
       </c>
       <c r="B133" s="9" t="s">
         <v>19</v>
@@ -2958,7 +3089,8 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" s="3">
-        <v>204</v>
+        <f t="shared" si="2"/>
+        <v>133</v>
       </c>
       <c r="B134" s="10" t="s">
         <v>79</v>
@@ -2972,7 +3104,8 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" s="3">
-        <v>205</v>
+        <f t="shared" si="2"/>
+        <v>134</v>
       </c>
       <c r="B135" s="9" t="s">
         <v>30</v>
@@ -2986,7 +3119,8 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" s="3">
-        <v>206</v>
+        <f t="shared" si="2"/>
+        <v>135</v>
       </c>
       <c r="B136" s="9" t="s">
         <v>18</v>
@@ -3000,7 +3134,8 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" s="3">
-        <v>207</v>
+        <f t="shared" si="2"/>
+        <v>136</v>
       </c>
       <c r="B137" s="10" t="s">
         <v>130</v>
@@ -3014,7 +3149,8 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" s="3">
-        <v>208</v>
+        <f t="shared" si="2"/>
+        <v>137</v>
       </c>
       <c r="B138" s="10" t="s">
         <v>154</v>
@@ -3028,7 +3164,8 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" s="3">
-        <v>209</v>
+        <f t="shared" si="2"/>
+        <v>138</v>
       </c>
       <c r="B139" s="9" t="s">
         <v>29</v>
@@ -3042,7 +3179,8 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" s="3">
-        <v>210</v>
+        <f t="shared" si="2"/>
+        <v>139</v>
       </c>
       <c r="B140" s="10" t="s">
         <v>176</v>
@@ -3056,7 +3194,8 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="3">
-        <v>211</v>
+        <f t="shared" si="2"/>
+        <v>140</v>
       </c>
       <c r="B141" s="10" t="s">
         <v>104</v>
@@ -3070,7 +3209,8 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="3">
-        <v>212</v>
+        <f t="shared" si="2"/>
+        <v>141</v>
       </c>
       <c r="B142" s="9" t="s">
         <v>41</v>
@@ -3084,7 +3224,8 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" s="3">
-        <v>213</v>
+        <f t="shared" si="2"/>
+        <v>142</v>
       </c>
       <c r="B143" s="9" t="s">
         <v>33</v>
@@ -3098,7 +3239,8 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" s="3">
-        <v>214</v>
+        <f t="shared" si="2"/>
+        <v>143</v>
       </c>
       <c r="B144" s="9" t="s">
         <v>15</v>
@@ -3112,7 +3254,8 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" s="3">
-        <v>215</v>
+        <f t="shared" si="2"/>
+        <v>144</v>
       </c>
       <c r="B145" s="10" t="s">
         <v>182</v>
@@ -3126,7 +3269,8 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" s="3">
-        <v>216</v>
+        <f t="shared" si="2"/>
+        <v>145</v>
       </c>
       <c r="B146" s="10" t="s">
         <v>167</v>
@@ -3140,7 +3284,8 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" s="3">
-        <v>217</v>
+        <f t="shared" si="2"/>
+        <v>146</v>
       </c>
       <c r="B147" s="10" t="s">
         <v>126</v>
@@ -3154,7 +3299,8 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" s="3">
-        <v>218</v>
+        <f t="shared" si="2"/>
+        <v>147</v>
       </c>
       <c r="B148" s="10" t="s">
         <v>123</v>
@@ -3168,7 +3314,8 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" s="3">
-        <v>219</v>
+        <f t="shared" si="2"/>
+        <v>148</v>
       </c>
       <c r="B149" s="10" t="s">
         <v>178</v>
@@ -3182,7 +3329,8 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" s="3">
-        <v>220</v>
+        <f t="shared" si="2"/>
+        <v>149</v>
       </c>
       <c r="B150" s="10" t="s">
         <v>155</v>
@@ -3196,7 +3344,8 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" s="3">
-        <v>221</v>
+        <f t="shared" si="2"/>
+        <v>150</v>
       </c>
       <c r="B151" s="10" t="s">
         <v>172</v>
@@ -3210,7 +3359,8 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" s="3">
-        <v>222</v>
+        <f t="shared" si="2"/>
+        <v>151</v>
       </c>
       <c r="B152" s="10" t="s">
         <v>133</v>
@@ -3224,7 +3374,8 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" s="3">
-        <v>223</v>
+        <f t="shared" si="2"/>
+        <v>152</v>
       </c>
       <c r="B153" s="10" t="s">
         <v>91</v>
@@ -3238,7 +3389,8 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" s="3">
-        <v>224</v>
+        <f t="shared" si="2"/>
+        <v>153</v>
       </c>
       <c r="B154" s="9" t="s">
         <v>51</v>
@@ -3252,7 +3404,8 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" s="3">
-        <v>225</v>
+        <f t="shared" si="2"/>
+        <v>154</v>
       </c>
       <c r="B155" s="10" t="s">
         <v>121</v>
@@ -3266,7 +3419,8 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" s="3">
-        <v>226</v>
+        <f t="shared" si="2"/>
+        <v>155</v>
       </c>
       <c r="B156" s="9" t="s">
         <v>47</v>
@@ -3280,7 +3434,8 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" s="3">
-        <v>227</v>
+        <f t="shared" si="2"/>
+        <v>156</v>
       </c>
       <c r="B157" s="10" t="s">
         <v>119</v>
@@ -3294,7 +3449,8 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" s="3">
-        <v>228</v>
+        <f t="shared" si="2"/>
+        <v>157</v>
       </c>
       <c r="B158" s="9" t="s">
         <v>11</v>
@@ -3308,7 +3464,8 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" s="3">
-        <v>229</v>
+        <f t="shared" si="2"/>
+        <v>158</v>
       </c>
       <c r="B159" s="10" t="s">
         <v>157</v>
@@ -3322,7 +3479,8 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" s="3">
-        <v>230</v>
+        <f t="shared" si="2"/>
+        <v>159</v>
       </c>
       <c r="B160" s="10" t="s">
         <v>127</v>
@@ -3336,7 +3494,8 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" s="3">
-        <v>231</v>
+        <f t="shared" si="2"/>
+        <v>160</v>
       </c>
       <c r="B161" s="10" t="s">
         <v>145</v>
@@ -3350,7 +3509,8 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" s="3">
-        <v>232</v>
+        <f t="shared" si="2"/>
+        <v>161</v>
       </c>
       <c r="B162" s="10" t="s">
         <v>183</v>
@@ -3364,7 +3524,8 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" s="3">
-        <v>233</v>
+        <f t="shared" si="2"/>
+        <v>162</v>
       </c>
       <c r="B163" s="10" t="s">
         <v>141</v>
@@ -3378,7 +3539,8 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" s="3">
-        <v>234</v>
+        <f t="shared" si="2"/>
+        <v>163</v>
       </c>
       <c r="B164" s="9" t="s">
         <v>23</v>
@@ -3392,7 +3554,8 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" s="3">
-        <v>235</v>
+        <f t="shared" si="2"/>
+        <v>164</v>
       </c>
       <c r="B165" s="10" t="s">
         <v>173</v>
@@ -3406,7 +3569,8 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" s="3">
-        <v>236</v>
+        <f t="shared" si="2"/>
+        <v>165</v>
       </c>
       <c r="B166" s="10" t="s">
         <v>161</v>
@@ -3420,7 +3584,8 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" s="3">
-        <v>237</v>
+        <f t="shared" si="2"/>
+        <v>166</v>
       </c>
       <c r="B167" s="10" t="s">
         <v>153</v>
@@ -3434,7 +3599,8 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" s="3">
-        <v>238</v>
+        <f t="shared" si="2"/>
+        <v>167</v>
       </c>
       <c r="B168" s="10" t="s">
         <v>149</v>
@@ -3448,7 +3614,8 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" s="3">
-        <v>239</v>
+        <f t="shared" si="2"/>
+        <v>168</v>
       </c>
       <c r="B169" s="10" t="s">
         <v>67</v>
@@ -3462,7 +3629,8 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" s="3">
-        <v>240</v>
+        <f t="shared" si="2"/>
+        <v>169</v>
       </c>
       <c r="B170" s="10" t="s">
         <v>156</v>
@@ -3476,7 +3644,8 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" s="3">
-        <v>241</v>
+        <f t="shared" si="2"/>
+        <v>170</v>
       </c>
       <c r="B171" s="10" t="s">
         <v>103</v>
@@ -3490,7 +3659,8 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" s="3">
-        <v>242</v>
+        <f t="shared" si="2"/>
+        <v>171</v>
       </c>
       <c r="B172" s="9" t="s">
         <v>53</v>
@@ -3504,7 +3674,8 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" s="3">
-        <v>243</v>
+        <f t="shared" si="2"/>
+        <v>172</v>
       </c>
       <c r="B173" s="9" t="s">
         <v>21</v>
@@ -3518,7 +3689,8 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" s="3">
-        <v>244</v>
+        <f t="shared" si="2"/>
+        <v>173</v>
       </c>
       <c r="B174" s="10" t="s">
         <v>151</v>
@@ -3532,7 +3704,8 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" s="3">
-        <v>245</v>
+        <f t="shared" si="2"/>
+        <v>174</v>
       </c>
       <c r="B175" s="9" t="s">
         <v>45</v>
@@ -3546,7 +3719,8 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" s="3">
-        <v>246</v>
+        <f t="shared" si="2"/>
+        <v>175</v>
       </c>
       <c r="B176" s="10" t="s">
         <v>179</v>
@@ -3560,7 +3734,8 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" s="3">
-        <v>247</v>
+        <f t="shared" si="2"/>
+        <v>176</v>
       </c>
       <c r="B177" s="10" t="s">
         <v>128</v>
@@ -3574,7 +3749,8 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" s="3">
-        <v>248</v>
+        <f t="shared" si="2"/>
+        <v>177</v>
       </c>
       <c r="B178" s="10" t="s">
         <v>180</v>
@@ -3588,7 +3764,8 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" s="3">
-        <v>249</v>
+        <f t="shared" si="2"/>
+        <v>178</v>
       </c>
       <c r="B179" s="9" t="s">
         <v>34</v>
@@ -3602,7 +3779,8 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" s="3">
-        <v>250</v>
+        <f t="shared" si="2"/>
+        <v>179</v>
       </c>
       <c r="B180" s="10" t="s">
         <v>168</v>
@@ -3616,7 +3794,8 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" s="3">
-        <v>251</v>
+        <f t="shared" si="2"/>
+        <v>180</v>
       </c>
       <c r="B181" s="9" t="s">
         <v>12</v>
@@ -3630,7 +3809,8 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" s="3">
-        <v>252</v>
+        <f t="shared" si="2"/>
+        <v>181</v>
       </c>
       <c r="B182" s="9" t="s">
         <v>25</v>
@@ -3644,7 +3824,8 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" s="3">
-        <v>253</v>
+        <f t="shared" si="2"/>
+        <v>182</v>
       </c>
       <c r="B183" s="10" t="s">
         <v>181</v>
@@ -3658,7 +3839,8 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" s="3">
-        <v>254</v>
+        <f t="shared" si="2"/>
+        <v>183</v>
       </c>
       <c r="B184" s="10" t="s">
         <v>184</v>
@@ -3672,7 +3854,8 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" s="3">
-        <v>255</v>
+        <f t="shared" si="2"/>
+        <v>184</v>
       </c>
       <c r="B185" s="10" t="s">
         <v>190</v>
@@ -3686,7 +3869,8 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" s="3">
-        <v>256</v>
+        <f t="shared" si="2"/>
+        <v>185</v>
       </c>
       <c r="B186" s="10" t="s">
         <v>120</v>
@@ -3700,7 +3884,8 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" s="3">
-        <v>257</v>
+        <f t="shared" si="2"/>
+        <v>186</v>
       </c>
       <c r="B187" s="10" t="s">
         <v>146</v>
@@ -3714,7 +3899,8 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" s="3">
-        <v>258</v>
+        <f t="shared" si="2"/>
+        <v>187</v>
       </c>
       <c r="B188" s="10" t="s">
         <v>196</v>
@@ -3728,7 +3914,8 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" s="3">
-        <v>259</v>
+        <f t="shared" si="2"/>
+        <v>188</v>
       </c>
       <c r="B189" s="10" t="s">
         <v>72</v>
@@ -3742,7 +3929,8 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" s="3">
-        <v>260</v>
+        <f t="shared" si="2"/>
+        <v>189</v>
       </c>
       <c r="B190" s="10" t="s">
         <v>147</v>
@@ -3756,7 +3944,8 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" s="3">
-        <v>261</v>
+        <f t="shared" si="2"/>
+        <v>190</v>
       </c>
       <c r="B191" s="10" t="s">
         <v>99</v>
@@ -3770,7 +3959,8 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" s="3">
-        <v>262</v>
+        <f t="shared" si="2"/>
+        <v>191</v>
       </c>
       <c r="B192" s="10" t="s">
         <v>85</v>
@@ -3784,7 +3974,8 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" s="3">
-        <v>173</v>
+        <f t="shared" si="2"/>
+        <v>192</v>
       </c>
       <c r="B193" s="9" t="s">
         <v>60</v>
@@ -3798,7 +3989,8 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" s="3">
-        <v>269</v>
+        <f t="shared" si="2"/>
+        <v>193</v>
       </c>
       <c r="B194" s="9" t="s">
         <v>63</v>
@@ -3812,7 +4004,8 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" s="3">
-        <v>270</v>
+        <f t="shared" si="2"/>
+        <v>194</v>
       </c>
       <c r="B195" s="9" t="s">
         <v>65</v>
@@ -3826,7 +4019,8 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" s="3">
-        <v>271</v>
+        <f t="shared" ref="A196:A201" si="3">A195+1</f>
+        <v>195</v>
       </c>
       <c r="B196" s="9" t="s">
         <v>59</v>
@@ -3840,7 +4034,8 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" s="3">
-        <v>306</v>
+        <f t="shared" si="3"/>
+        <v>196</v>
       </c>
       <c r="B197" s="9" t="s">
         <v>62</v>
@@ -3854,7 +4049,8 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" s="3">
-        <v>1293</v>
+        <f t="shared" si="3"/>
+        <v>197</v>
       </c>
       <c r="B198" s="9" t="s">
         <v>66</v>
@@ -3868,7 +4064,8 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" s="3">
-        <v>1295</v>
+        <f t="shared" si="3"/>
+        <v>198</v>
       </c>
       <c r="B199" s="9" t="s">
         <v>58</v>
@@ -3882,7 +4079,8 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" s="3">
-        <v>1450</v>
+        <f t="shared" si="3"/>
+        <v>199</v>
       </c>
       <c r="B200" s="9" t="s">
         <v>64</v>
@@ -3896,7 +4094,8 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" s="3">
-        <v>1459</v>
+        <f t="shared" si="3"/>
+        <v>200</v>
       </c>
       <c r="B201" s="9" t="s">
         <v>61</v>

</xml_diff>